<commit_message>
Bugs fix, Definisions fix and run test
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cory8\OneDrive\Documents\UiPath\MiniBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{4C6F0680-7CBF-4976-9863-5109C4AA17F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{589A81CE-992E-477B-B2AA-0DBD323F2716}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{4C6F0680-7CBF-4976-9863-5109C4AA17F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6AE69075-D786-4267-B9C2-8978247EAF25}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>Output_FilePath</t>
+  </si>
+  <si>
+    <t>C:\Users\Cory8\OneDrive\Documents\UiPath\MiniBot\Data\Weather.txt</t>
+  </si>
+  <si>
+    <t>C:\Users\Cory8\OneDrive\Documents\UiPath\MiniBot\Data\MiniBot_Input.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1572,7 +1578,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1701,10 +1707,16 @@
       <c r="A12" t="s">
         <v>30</v>
       </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
         <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>